<commit_message>
Adding percentage data to Lab 15
</commit_message>
<xml_diff>
--- a/15_a_normal_meal/15_a_normal_meal_data.xlsx
+++ b/15_a_normal_meal/15_a_normal_meal_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
   <si>
     <t>Glucose Mass(mg)*</t>
   </si>
@@ -88,13 +88,19 @@
   </si>
   <si>
     <t>Fat Trigly Uptake is not given under triglyceride metabolism so I’m using the gain in the balance box</t>
+  </si>
+  <si>
+    <t>% Diff</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +131,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -202,10 +215,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
@@ -221,11 +235,58 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -515,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1537,7 +1598,571 @@
       <c r="M43" s="6"/>
       <c r="N43" s="6"/>
     </row>
+    <row r="44" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="45" spans="1:14" ht="24" thickBot="1">
+      <c r="A45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="I45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A46" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="7">
+        <f>ABS((B2-B20)/B2)</f>
+        <v>1.3523316062176119E-2</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="7">
+        <f t="shared" ref="C46:H46" si="0">ABS((D2-D20)/D2)</f>
+        <v>5.8727788562042776E-2</v>
+      </c>
+      <c r="E46" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5542919378941703E-2</v>
+      </c>
+      <c r="F46" s="7">
+        <f t="shared" si="0"/>
+        <v>6.7637716362895173E-2</v>
+      </c>
+      <c r="G46" s="7">
+        <f t="shared" si="0"/>
+        <v>0.1601416114564124</v>
+      </c>
+      <c r="H46" s="7">
+        <f t="shared" si="0"/>
+        <v>0.82115205056381524</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="7">
+        <f t="shared" ref="B47:H47" si="1">ABS((B3-B21)/B3)</f>
+        <v>1.3316582914572864E-2</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="7">
+        <f t="shared" si="1"/>
+        <v>1.1154172217512458E-2</v>
+      </c>
+      <c r="E47" s="7">
+        <f t="shared" si="1"/>
+        <v>1.1679999999999975E-2</v>
+      </c>
+      <c r="F47" s="7">
+        <f t="shared" si="1"/>
+        <v>1.2122494314275175E-2</v>
+      </c>
+      <c r="G47" s="7">
+        <f t="shared" si="1"/>
+        <v>2.2700663457785871E-2</v>
+      </c>
+      <c r="H47" s="7">
+        <f t="shared" si="1"/>
+        <v>4.3587726199842712E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A48" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="7">
+        <f t="shared" ref="B48:H48" si="2">ABS((B4-B22)/B4)</f>
+        <v>1.6124999999999973E-2</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="7">
+        <f t="shared" si="2"/>
+        <v>8.2189054726368518E-3</v>
+      </c>
+      <c r="E48" s="7">
+        <f t="shared" si="2"/>
+        <v>9.903381642512055E-3</v>
+      </c>
+      <c r="F48" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1278536511616151E-2</v>
+      </c>
+      <c r="G48" s="7">
+        <f t="shared" si="2"/>
+        <v>4.0853658536585284E-2</v>
+      </c>
+      <c r="H48" s="7">
+        <f t="shared" si="2"/>
+        <v>9.5000000000000029E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="7">
+        <f t="shared" ref="B49:H49" si="3">ABS((B5-B23)/B5)</f>
+        <v>7.6146788990825665E-2</v>
+      </c>
+      <c r="C49" s="7">
+        <f t="shared" si="3"/>
+        <v>0.13164556962025323</v>
+      </c>
+      <c r="D49" s="7">
+        <f t="shared" si="3"/>
+        <v>1.8947368421052602E-2</v>
+      </c>
+      <c r="E49" s="7">
+        <f t="shared" si="3"/>
+        <v>8.8181818181818208E-2</v>
+      </c>
+      <c r="F49" s="7">
+        <f t="shared" si="3"/>
+        <v>8.9075630252100788E-2</v>
+      </c>
+      <c r="G49" s="7">
+        <f t="shared" si="3"/>
+        <v>5.5645161290322626E-2</v>
+      </c>
+      <c r="H49" s="7">
+        <f t="shared" si="3"/>
+        <v>0.36153846153846159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="7">
+        <f t="shared" ref="B50:H50" si="4">ABS((B6-B24)/B6)</f>
+        <v>0.12333333333333327</v>
+      </c>
+      <c r="C50" s="7">
+        <f t="shared" si="4"/>
+        <v>0.1247524752475247</v>
+      </c>
+      <c r="D50" s="7">
+        <f t="shared" si="4"/>
+        <v>0.21111111111111108</v>
+      </c>
+      <c r="E50" s="7">
+        <f t="shared" si="4"/>
+        <v>0.27155172413793105</v>
+      </c>
+      <c r="F50" s="7">
+        <f t="shared" si="4"/>
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="G50" s="7">
+        <f t="shared" si="4"/>
+        <v>0.47551020408163269</v>
+      </c>
+      <c r="H50" s="7">
+        <f t="shared" si="4"/>
+        <v>0.32033898305084746</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="7">
+        <f t="shared" ref="B51:H51" si="5">ABS((B7-B25)/B7)</f>
+        <v>0.13430127041742285</v>
+      </c>
+      <c r="C51" s="7">
+        <f t="shared" si="5"/>
+        <v>0.12345679012345678</v>
+      </c>
+      <c r="D51" s="7">
+        <f t="shared" si="5"/>
+        <v>0.11858407079646023</v>
+      </c>
+      <c r="E51" s="7">
+        <f t="shared" si="5"/>
+        <v>0.11858407079646023</v>
+      </c>
+      <c r="F51" s="7">
+        <f t="shared" si="5"/>
+        <v>0.1203539823008849</v>
+      </c>
+      <c r="G51" s="7">
+        <f t="shared" si="5"/>
+        <v>0.13005272407732862</v>
+      </c>
+      <c r="H51" s="7">
+        <f t="shared" si="5"/>
+        <v>4.4859813084112125E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A52" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="7">
+        <f t="shared" ref="B52:H52" si="6">ABS((B8-B26)/B8)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="C52" s="7">
+        <f t="shared" si="6"/>
+        <v>0.36363636363636354</v>
+      </c>
+      <c r="D52" s="7">
+        <f t="shared" si="6"/>
+        <v>0.1538461538461538</v>
+      </c>
+      <c r="E52" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="7">
+        <f t="shared" si="6"/>
+        <v>0.17647058823529416</v>
+      </c>
+      <c r="G52" s="7">
+        <f t="shared" si="6"/>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="H52" s="7">
+        <f t="shared" si="6"/>
+        <v>8.3333333333333232E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="7">
+        <f t="shared" ref="B53:H53" si="7">ABS((B9-B27)/B9)</f>
+        <v>0.22368421052631571</v>
+      </c>
+      <c r="C53" s="7">
+        <f t="shared" si="7"/>
+        <v>0.49650349650349651</v>
+      </c>
+      <c r="D53" s="7">
+        <f t="shared" si="7"/>
+        <v>0.55688622754491013</v>
+      </c>
+      <c r="E53" s="7">
+        <f t="shared" si="7"/>
+        <v>0.61340206185567003</v>
+      </c>
+      <c r="F53" s="7">
+        <f t="shared" si="7"/>
+        <v>0.6919642857142857</v>
+      </c>
+      <c r="G53" s="7">
+        <f t="shared" si="7"/>
+        <v>0.81605351170568563</v>
+      </c>
+      <c r="H53" s="7">
+        <f t="shared" si="7"/>
+        <v>0.77327935222672073</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="7">
+        <f t="shared" ref="B54:H54" si="8">ABS((B10-B28)/B10)</f>
+        <v>5.6250000000000022E-2</v>
+      </c>
+      <c r="C54" s="7">
+        <f t="shared" si="8"/>
+        <v>5.4545454545454515E-2</v>
+      </c>
+      <c r="D54" s="7">
+        <f t="shared" si="8"/>
+        <v>5.4545454545454515E-2</v>
+      </c>
+      <c r="E54" s="7">
+        <f t="shared" si="8"/>
+        <v>0.10909090909090903</v>
+      </c>
+      <c r="F54" s="7">
+        <f t="shared" si="8"/>
+        <v>0.44000000000000006</v>
+      </c>
+      <c r="G54" s="7">
+        <f t="shared" si="8"/>
+        <v>2.1857142857142859</v>
+      </c>
+      <c r="H54" s="7">
+        <f t="shared" si="8"/>
+        <v>0.82727272727272738</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A55" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="7">
+        <f t="shared" ref="B55:H55" si="9">ABS((B11-B29)/B11)</f>
+        <v>6.3636363636363574E-2</v>
+      </c>
+      <c r="C55" s="7">
+        <f t="shared" si="9"/>
+        <v>0.24909090909090914</v>
+      </c>
+      <c r="D55" s="7">
+        <f t="shared" si="9"/>
+        <v>0.21588785046728967</v>
+      </c>
+      <c r="E55" s="7">
+        <f t="shared" si="9"/>
+        <v>0.1864077669902913</v>
+      </c>
+      <c r="F55" s="7">
+        <f t="shared" si="9"/>
+        <v>0.14646464646464646</v>
+      </c>
+      <c r="G55" s="7">
+        <f t="shared" si="9"/>
+        <v>7.1739130434782541E-2</v>
+      </c>
+      <c r="H55" s="7">
+        <f t="shared" si="9"/>
+        <v>0.35874125874125873</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A56" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="7">
+        <f t="shared" ref="B56:H56" si="10">ABS((B12-B30)/B12)</f>
+        <v>0.12030075187969921</v>
+      </c>
+      <c r="C56" s="7">
+        <f t="shared" si="10"/>
+        <v>0.56986301369863013</v>
+      </c>
+      <c r="D56" s="7">
+        <f t="shared" si="10"/>
+        <v>0.55932203389830504</v>
+      </c>
+      <c r="E56" s="7">
+        <f t="shared" si="10"/>
+        <v>0.55102040816326536</v>
+      </c>
+      <c r="F56" s="7">
+        <f t="shared" si="10"/>
+        <v>0.52727272727272723</v>
+      </c>
+      <c r="G56" s="7">
+        <f t="shared" si="10"/>
+        <v>0.47368421052631576</v>
+      </c>
+      <c r="H56" s="7">
+        <f t="shared" si="10"/>
+        <v>0.70529801324503305</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="7">
+        <f t="shared" ref="B57:H57" si="11">ABS((B13-B31)/B13)</f>
+        <v>0.23292682926829261</v>
+      </c>
+      <c r="C57" s="7">
+        <f t="shared" si="11"/>
+        <v>0.69166666666666676</v>
+      </c>
+      <c r="D57" s="7">
+        <f t="shared" si="11"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="E57" s="7">
+        <f t="shared" si="11"/>
+        <v>0.44464285714285723</v>
+      </c>
+      <c r="F57" s="7">
+        <f t="shared" si="11"/>
+        <v>0.29777777777777775</v>
+      </c>
+      <c r="G57" s="7">
+        <f t="shared" si="11"/>
+        <v>5.83850931677019E-2</v>
+      </c>
+      <c r="H57" s="7">
+        <f t="shared" si="11"/>
+        <v>3.5031847133757961E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A58" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="7">
+        <f t="shared" ref="B58:H58" si="12">ABS((B14-B32)/B14)</f>
+        <v>0.25853658536585367</v>
+      </c>
+      <c r="C58" s="7">
+        <f t="shared" si="12"/>
+        <v>0.60588235294117654</v>
+      </c>
+      <c r="D58" s="7">
+        <f t="shared" si="12"/>
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="E58" s="7">
+        <f t="shared" si="12"/>
+        <v>7.9591836734693847E-2</v>
+      </c>
+      <c r="F58" s="7">
+        <f t="shared" si="12"/>
+        <v>0.6461538461538463</v>
+      </c>
+      <c r="G58" s="7">
+        <f t="shared" si="12"/>
+        <v>0.47700534759358282</v>
+      </c>
+      <c r="H58" s="7">
+        <f t="shared" si="12"/>
+        <v>1.71340206185567</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A59" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="7">
+        <f t="shared" ref="B59:H59" si="13">ABS((B15-B33)/B15)</f>
+        <v>0.13700000000000004</v>
+      </c>
+      <c r="C59" s="7">
+        <f t="shared" si="13"/>
+        <v>0.23432835820895526</v>
+      </c>
+      <c r="D59" s="7">
+        <f t="shared" si="13"/>
+        <v>0.25588235294117656</v>
+      </c>
+      <c r="E59" s="7">
+        <f t="shared" si="13"/>
+        <v>0.28115942028985513</v>
+      </c>
+      <c r="F59" s="7">
+        <f t="shared" si="13"/>
+        <v>0.30285714285714288</v>
+      </c>
+      <c r="G59" s="7">
+        <f t="shared" si="13"/>
+        <v>0.30263157894736842</v>
+      </c>
+      <c r="H59" s="7">
+        <f t="shared" si="13"/>
+        <v>0.46052631578947367</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A60" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="7">
+        <f t="shared" ref="B60:H60" si="14">ABS((B16-B34)/B16)</f>
+        <v>5.0505050505050504E-2</v>
+      </c>
+      <c r="C60" s="7">
+        <f t="shared" si="14"/>
+        <v>0.66964285714285721</v>
+      </c>
+      <c r="D60" s="7">
+        <f t="shared" si="14"/>
+        <v>0.52845528455284552</v>
+      </c>
+      <c r="E60" s="7">
+        <f t="shared" si="14"/>
+        <v>0.21875</v>
+      </c>
+      <c r="F60" s="7">
+        <f t="shared" si="14"/>
+        <v>9.8039215686275914E-3</v>
+      </c>
+      <c r="G60" s="7">
+        <f t="shared" si="14"/>
+        <v>7.0312499999999889E-2</v>
+      </c>
+      <c r="H60" s="7">
+        <f t="shared" si="14"/>
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A61" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="7">
+        <f t="shared" ref="B61:H61" si="15">ABS((B17-B35)/B17)</f>
+        <v>2.8985507246377224E-3</v>
+      </c>
+      <c r="C61" s="7">
+        <f t="shared" si="15"/>
+        <v>0.15294117647058825</v>
+      </c>
+      <c r="D61" s="7">
+        <f t="shared" si="15"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="E61" s="7">
+        <f t="shared" si="15"/>
+        <v>0.11851851851851845</v>
+      </c>
+      <c r="F61" s="7">
+        <f t="shared" si="15"/>
+        <v>7.3684210526315713E-2</v>
+      </c>
+      <c r="G61" s="7">
+        <f t="shared" si="15"/>
+        <v>5.9701492537314283E-3</v>
+      </c>
+      <c r="H61" s="7">
+        <f t="shared" si="15"/>
+        <v>0.38125000000000003</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B46:H61">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>